<commit_message>
Fixed missing workflow_istance_id for 448 & 449
</commit_message>
<xml_diff>
--- a/GATEWAY/A1#111#MEDICALCLOUDSRLX4/medicalcloud/visitasmart/1.0/report-checklist_V8.2.5_Medicalcloud_New.xlsx
+++ b/GATEWAY/A1#111#MEDICALCLOUDSRLX4/medicalcloud/visitasmart/1.0/report-checklist_V8.2.5_Medicalcloud_New.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosar\Desktop\giovanni\medical cloud\FSE 2.0\test uff\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1927B52-72B1-42AE-AFFF-26D6726D2295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE4BF262-F02A-4787-B9DA-EA2003E9127F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{C39DE83B-1739-445D-8950-88F749A314C1}"/>
   </bookViews>
@@ -7320,25 +7320,25 @@
     <t>2.16.840.1.113883.2.9.2.190.4.4.82a76523b4cdbf22bec6e25e8561d71e179f3e3f762a68ae716381f2293e70e5.88bd80541e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2025-05-14T09:01:38Z</t>
-  </si>
-  <si>
-    <t>f70496bf46c0e1477b8007b00a7f383b</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.82a76523b4cdbf22bec6e25e8561d71e179f3e3f762a68ae716381f2293e70e5.e2f658e4c0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2025-05-14T09:21:00Z</t>
-  </si>
-  <si>
-    <t>f0b94415ce7f7ef97eb928b111f309c1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.190.4.4.82a76523b4cdbf22bec6e25e8561d71e179f3e3f762a68ae716381f2293e70e5.de4bd43262^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>Il sistema rileva in fase di validazione l’assenza del codice che specifica il grado di parentela. L’errore è visibile all’utente, che deve completare l’anamnesi familiare con l’informazione mancante e procedere con un nuovo invio.</t>
+  </si>
+  <si>
+    <t>2025-05-15T08:22:17Z</t>
+  </si>
+  <si>
+    <t>86a0662ef21027a1d4325180b5714136</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.82a76523b4cdbf22bec6e25e8561d71e179f3e3f762a68ae716381f2293e70e5.e7832d52e1^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2025-05-15T08:32:35Z</t>
+  </si>
+  <si>
+    <t>3b6902ecb430c3339afffda98d3b81bb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.190.4.4.82a76523b4cdbf22bec6e25e8561d71e179f3e3f762a68ae716381f2293e70e5.b15b3a3611^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -9290,8 +9290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE1845C-3E9D-4496-B772-E13496BB4925}">
   <dimension ref="A1:AMJ755"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q4" workbookViewId="0">
-      <selection activeCell="S129" sqref="S129"/>
+    <sheetView tabSelected="1" topLeftCell="F4" workbookViewId="0">
+      <selection activeCell="I170" sqref="I170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -14383,7 +14383,7 @@
         <v>63</v>
       </c>
       <c r="S129" s="34" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="T129" s="27"/>
       <c r="U129" s="28"/>
@@ -15948,16 +15948,16 @@
         <v>374</v>
       </c>
       <c r="F169" s="32">
-        <v>45791</v>
+        <v>45792</v>
       </c>
       <c r="G169" s="33" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="H169" s="33" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="I169" s="2" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="J169" s="27" t="s">
         <v>63</v>
@@ -15995,16 +15995,16 @@
         <v>376</v>
       </c>
       <c r="F170" s="32">
-        <v>45791</v>
+        <v>45792</v>
       </c>
       <c r="G170" s="33" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="H170" s="33" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="I170" s="2" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="J170" s="27" t="s">
         <v>63</v>

</xml_diff>